<commit_message>
melhorias no tratamento das mensagens de erro retornados pela API Microwork
</commit_message>
<xml_diff>
--- a/indicadores/veiculos_vendas.xlsx
+++ b/indicadores/veiculos_vendas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U359"/>
+  <dimension ref="A1:U360"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -33690,6 +33690,99 @@
         <v>-4.9389</v>
       </c>
     </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>MMA</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>VENDA</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>NF-E 9804050/890</t>
+        </is>
+      </c>
+      <c r="D360" t="inlineStr">
+        <is>
+          <t>2025-05-08T00:00:00</t>
+        </is>
+      </c>
+      <c r="E360" t="inlineStr">
+        <is>
+          <t>2025-05-13T00:00:00</t>
+        </is>
+      </c>
+      <c r="F360" t="inlineStr">
+        <is>
+          <t>NF-E 156980/1</t>
+        </is>
+      </c>
+      <c r="G360" t="inlineStr">
+        <is>
+          <t>2025-08-26T14:55:08</t>
+        </is>
+      </c>
+      <c r="H360" t="n">
+        <v>1</v>
+      </c>
+      <c r="I360" t="n">
+        <v>1132</v>
+      </c>
+      <c r="J360" t="inlineStr">
+        <is>
+          <t>AXOR 2044 S</t>
+        </is>
+      </c>
+      <c r="K360" t="inlineStr">
+        <is>
+          <t>BRANCA</t>
+        </is>
+      </c>
+      <c r="L360" t="inlineStr">
+        <is>
+          <t>2010/2011</t>
+        </is>
+      </c>
+      <c r="M360" t="inlineStr">
+        <is>
+          <t>TRANSPORTADORA RODOVIARIA DE CARGAS MODENA LTDA</t>
+        </is>
+      </c>
+      <c r="N360" t="n">
+        <v>855</v>
+      </c>
+      <c r="O360" t="inlineStr">
+        <is>
+          <t>RAPHAELA GALVÃO DE SOUZA</t>
+        </is>
+      </c>
+      <c r="P360" t="inlineStr">
+        <is>
+          <t>AV - À VISTA</t>
+        </is>
+      </c>
+      <c r="Q360" t="n">
+        <v>23940</v>
+      </c>
+      <c r="R360" t="inlineStr">
+        <is>
+          <t>LUDVIG STOCKL</t>
+        </is>
+      </c>
+      <c r="S360" t="n">
+        <v>159440</v>
+      </c>
+      <c r="T360" t="n">
+        <v>-560</v>
+      </c>
+      <c r="U360" t="n">
+        <v>-0.3512</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>